<commit_message>
Vlada v2, import fixed
</commit_message>
<xml_diff>
--- a/cene.xlsx
+++ b/cene.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\intersocks.com\files\users\milos.radojkovic\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milos.radojkovic\Documents\Python\Evidencija plaćanja zaduženja _old\Evidencija-placanja-zaduzenja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9A96E7-EA48-4521-BDEA-423555C49C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4770D1-E360-499A-826E-BBFF7EE87E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2148" yWindow="3312" windowWidth="17280" windowHeight="8928" xr2:uid="{D7A55D32-58E7-42F2-90F1-9005A34C25E2}"/>
   </bookViews>
@@ -3016,7 +3016,7 @@
   <dimension ref="A1:F696"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F696"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3056,7 +3056,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>268</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -3076,7 +3076,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>269</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3096,7 +3096,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E4">
         <v>0</v>

</xml_diff>